<commit_message>
full tables without koeffs
</commit_message>
<xml_diff>
--- a/tables/balans_obschiy.xlsx
+++ b/tables/balans_obschiy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RGR_Economy_Analis\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028F3F1A-AED4-4BE6-8700-D5CC990F0BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A372B2-F90A-4878-9C9F-8B7B7D6225C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59468F68-95C9-43AE-BBC8-B50A8E0C9D40}"/>
+    <workbookView xWindow="12444" yWindow="576" windowWidth="10332" windowHeight="10884" activeTab="1" xr2:uid="{59468F68-95C9-43AE-BBC8-B50A8E0C9D40}"/>
   </bookViews>
   <sheets>
     <sheet name="форма1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="338">
   <si>
     <t xml:space="preserve">                                                                                </t>
   </si>
@@ -1046,7 +1046,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,11 +1104,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
     <font>
@@ -1227,7 +1222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1253,37 +1248,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1299,25 +1294,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1329,38 +1327,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1684,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC41E0A9-EA75-450C-AE30-7FDBD041BE34}">
   <dimension ref="A1:F1198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1952,25 +1941,25 @@
     <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -1980,22 +1969,22 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2009,78 +1998,78 @@
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="38">
         <v>200007197</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -2098,14 +2087,14 @@
     </row>
     <row r="20" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="30"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="1"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="30"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="1"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
@@ -2132,17 +2121,17 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
     </row>
     <row r="26" spans="1:6" ht="24.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="9" t="s">
         <v>19</v>
       </c>
@@ -2175,20 +2164,20 @@
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="39"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="13" t="s">
         <v>28</v>
       </c>
@@ -2203,10 +2192,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="39"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="13" t="s">
         <v>32</v>
       </c>
@@ -2221,10 +2210,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="40"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="11" t="s">
         <v>36</v>
       </c>
@@ -2237,20 +2226,20 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="13"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="13" t="s">
         <v>39</v>
       </c>
@@ -2263,10 +2252,10 @@
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="13" t="s">
         <v>41</v>
       </c>
@@ -2279,10 +2268,10 @@
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="13" t="s">
         <v>43</v>
       </c>
@@ -2295,10 +2284,10 @@
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="13" t="s">
         <v>45</v>
       </c>
@@ -2313,10 +2302,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="39"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="13" t="s">
         <v>49</v>
       </c>
@@ -2331,10 +2320,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="13" t="s">
         <v>51</v>
       </c>
@@ -2347,10 +2336,10 @@
       <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="39"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="13" t="s">
         <v>53</v>
       </c>
@@ -2363,10 +2352,10 @@
       <c r="F39" s="22"/>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="39"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="13" t="s">
         <v>56</v>
       </c>
@@ -2379,10 +2368,10 @@
       <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="39"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="13" t="s">
         <v>58</v>
       </c>
@@ -2397,10 +2386,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="11" t="s">
         <v>61</v>
       </c>
@@ -2415,20 +2404,20 @@
       </c>
     </row>
     <row r="43" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="40"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="11"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="40"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="11" t="s">
         <v>66</v>
       </c>
@@ -2443,20 +2432,20 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="39"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="13"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="24"/>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="39"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="13" t="s">
         <v>70</v>
       </c>
@@ -2471,10 +2460,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="13" t="s">
         <v>74</v>
       </c>
@@ -2489,10 +2478,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="39"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="13" t="s">
         <v>76</v>
       </c>
@@ -2507,10 +2496,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="39"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="13" t="s">
         <v>80</v>
       </c>
@@ -2525,10 +2514,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="39"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="13" t="s">
         <v>84</v>
       </c>
@@ -2543,10 +2532,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="39"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="13" t="s">
         <v>86</v>
       </c>
@@ -2561,10 +2550,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="39"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="13" t="s">
         <v>88</v>
       </c>
@@ -2579,10 +2568,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="39"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="13" t="s">
         <v>90</v>
       </c>
@@ -2597,10 +2586,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B54" s="39"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="13" t="s">
         <v>94</v>
       </c>
@@ -2615,10 +2604,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B55" s="39"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="13" t="s">
         <v>98</v>
       </c>
@@ -2633,10 +2622,10 @@
       </c>
     </row>
     <row r="56" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="39"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="13" t="s">
         <v>101</v>
       </c>
@@ -2649,10 +2638,10 @@
       <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="39"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="13" t="s">
         <v>103</v>
       </c>
@@ -2665,10 +2654,10 @@
       <c r="F57" s="22"/>
     </row>
     <row r="58" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="39"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="13" t="s">
         <v>105</v>
       </c>
@@ -2683,10 +2672,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="39"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="13" t="s">
         <v>109</v>
       </c>
@@ -2701,10 +2690,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="40" t="s">
+      <c r="A60" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="40"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="11" t="s">
         <v>112</v>
       </c>
@@ -2719,10 +2708,10 @@
       </c>
     </row>
     <row r="61" spans="1:6" s="2" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="40"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="11" t="s">
         <v>116</v>
       </c>
@@ -2737,10 +2726,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" s="2" customFormat="1" ht="24.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="41" t="s">
+      <c r="A62" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="41"/>
+      <c r="B62" s="34"/>
       <c r="C62" s="15" t="s">
         <v>19</v>
       </c>
@@ -2773,20 +2762,20 @@
       </c>
     </row>
     <row r="64" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B64" s="40"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="11"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="22"/>
     </row>
     <row r="65" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="39"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="13" t="s">
         <v>121</v>
       </c>
@@ -2801,10 +2790,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="39" t="s">
+      <c r="A66" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="39"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="13" t="s">
         <v>124</v>
       </c>
@@ -2819,10 +2808,10 @@
       </c>
     </row>
     <row r="67" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B67" s="39"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="13" t="s">
         <v>126</v>
       </c>
@@ -2837,10 +2826,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="39"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="13" t="s">
         <v>128</v>
       </c>
@@ -2855,10 +2844,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="39" t="s">
+      <c r="A69" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="39"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="13" t="s">
         <v>131</v>
       </c>
@@ -2873,10 +2862,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="39" t="s">
+      <c r="A70" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="B70" s="39"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="13" t="s">
         <v>135</v>
       </c>
@@ -2891,10 +2880,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B71" s="39"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="13" t="s">
         <v>139</v>
       </c>
@@ -2909,10 +2898,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="39" t="s">
+      <c r="A72" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="39"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="13" t="s">
         <v>141</v>
       </c>
@@ -2927,10 +2916,10 @@
       </c>
     </row>
     <row r="73" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="40" t="s">
+      <c r="A73" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B73" s="40"/>
+      <c r="B73" s="28"/>
       <c r="C73" s="11" t="s">
         <v>143</v>
       </c>
@@ -2945,20 +2934,20 @@
       </c>
     </row>
     <row r="74" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="40" t="s">
+      <c r="A74" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="40"/>
+      <c r="B74" s="28"/>
       <c r="C74" s="11"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="24"/>
     </row>
     <row r="75" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="39"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="13" t="s">
         <v>148</v>
       </c>
@@ -2973,10 +2962,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="39" t="s">
+      <c r="A76" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="B76" s="39"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="13" t="s">
         <v>152</v>
       </c>
@@ -2991,10 +2980,10 @@
       </c>
     </row>
     <row r="77" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="39" t="s">
+      <c r="A77" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="B77" s="39"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="13" t="s">
         <v>154</v>
       </c>
@@ -3009,10 +2998,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="39" t="s">
+      <c r="A78" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="39"/>
+      <c r="B78" s="31"/>
       <c r="C78" s="13" t="s">
         <v>156</v>
       </c>
@@ -3027,10 +3016,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="39"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="13" t="s">
         <v>159</v>
       </c>
@@ -3045,10 +3034,10 @@
       </c>
     </row>
     <row r="80" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="B80" s="39"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="13" t="s">
         <v>34</v>
       </c>
@@ -3063,10 +3052,10 @@
       </c>
     </row>
     <row r="81" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="40" t="s">
+      <c r="A81" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B81" s="40"/>
+      <c r="B81" s="28"/>
       <c r="C81" s="11" t="s">
         <v>162</v>
       </c>
@@ -3081,20 +3070,20 @@
       </c>
     </row>
     <row r="82" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="40" t="s">
+      <c r="A82" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="B82" s="40"/>
+      <c r="B82" s="28"/>
       <c r="C82" s="11"/>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
       <c r="F82" s="24"/>
     </row>
     <row r="83" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="39" t="s">
+      <c r="A83" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B83" s="39"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="13" t="s">
         <v>167</v>
       </c>
@@ -3109,10 +3098,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B84" s="39"/>
+      <c r="B84" s="31"/>
       <c r="C84" s="13" t="s">
         <v>171</v>
       </c>
@@ -3127,10 +3116,10 @@
       </c>
     </row>
     <row r="85" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="40" t="s">
+      <c r="A85" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="B85" s="40"/>
+      <c r="B85" s="28"/>
       <c r="C85" s="11" t="s">
         <v>175</v>
       </c>
@@ -3145,20 +3134,20 @@
       </c>
     </row>
     <row r="86" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="39" t="s">
+      <c r="A86" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="39"/>
+      <c r="B86" s="31"/>
       <c r="C86" s="13"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="24"/>
     </row>
     <row r="87" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B87" s="39"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="13" t="s">
         <v>179</v>
       </c>
@@ -3173,10 +3162,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="39" t="s">
+      <c r="A88" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="B88" s="39"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="13" t="s">
         <v>183</v>
       </c>
@@ -3191,10 +3180,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="39" t="s">
+      <c r="A89" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="B89" s="39"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="13" t="s">
         <v>187</v>
       </c>
@@ -3209,10 +3198,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="39" t="s">
+      <c r="A90" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B90" s="39"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="13" t="s">
         <v>191</v>
       </c>
@@ -3227,10 +3216,10 @@
       </c>
     </row>
     <row r="91" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="B91" s="39"/>
+      <c r="B91" s="31"/>
       <c r="C91" s="13" t="s">
         <v>195</v>
       </c>
@@ -3245,10 +3234,10 @@
       </c>
     </row>
     <row r="92" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="39" t="s">
+      <c r="A92" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="B92" s="39"/>
+      <c r="B92" s="31"/>
       <c r="C92" s="13" t="s">
         <v>199</v>
       </c>
@@ -3263,10 +3252,10 @@
       </c>
     </row>
     <row r="93" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="39" t="s">
+      <c r="A93" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B93" s="39"/>
+      <c r="B93" s="31"/>
       <c r="C93" s="13" t="s">
         <v>201</v>
       </c>
@@ -3281,10 +3270,10 @@
       </c>
     </row>
     <row r="94" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="B94" s="39"/>
+      <c r="B94" s="31"/>
       <c r="C94" s="13" t="s">
         <v>203</v>
       </c>
@@ -3299,10 +3288,10 @@
       </c>
     </row>
     <row r="95" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="42" t="s">
+      <c r="A95" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="B95" s="42"/>
+      <c r="B95" s="32"/>
       <c r="C95" s="13" t="s">
         <v>207</v>
       </c>
@@ -3317,10 +3306,10 @@
       </c>
     </row>
     <row r="96" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="B96" s="39"/>
+      <c r="B96" s="31"/>
       <c r="C96" s="13" t="s">
         <v>208</v>
       </c>
@@ -3335,10 +3324,10 @@
       </c>
     </row>
     <row r="97" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="39" t="s">
+      <c r="A97" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="B97" s="39"/>
+      <c r="B97" s="31"/>
       <c r="C97" s="13" t="s">
         <v>209</v>
       </c>
@@ -3353,10 +3342,10 @@
       </c>
     </row>
     <row r="98" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="39" t="s">
+      <c r="A98" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="B98" s="39"/>
+      <c r="B98" s="31"/>
       <c r="C98" s="13" t="s">
         <v>211</v>
       </c>
@@ -3371,10 +3360,10 @@
       </c>
     </row>
     <row r="99" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="40" t="s">
+      <c r="A99" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B99" s="40"/>
+      <c r="B99" s="28"/>
       <c r="C99" s="11" t="s">
         <v>213</v>
       </c>
@@ -3389,10 +3378,10 @@
       </c>
     </row>
     <row r="100" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="40" t="s">
+      <c r="A100" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="B100" s="40"/>
+      <c r="B100" s="28"/>
       <c r="C100" s="11" t="s">
         <v>217</v>
       </c>
@@ -3407,29 +3396,29 @@
       </c>
     </row>
     <row r="101" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="43"/>
-      <c r="B101" s="43"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
       <c r="C101" s="16"/>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
     </row>
     <row r="102" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="44"/>
-      <c r="B102" s="44"/>
-      <c r="C102" s="44"/>
-      <c r="D102" s="45"/>
-      <c r="E102" s="45"/>
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="30"/>
     </row>
     <row r="103" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="44"/>
-      <c r="B103" s="44"/>
-      <c r="C103" s="44"/>
-      <c r="D103" s="45"/>
-      <c r="E103" s="45"/>
+      <c r="A103" s="29"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="30"/>
+      <c r="E103" s="30"/>
     </row>
     <row r="104" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="43"/>
-      <c r="B104" s="43"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
       <c r="C104" s="16"/>
       <c r="D104" s="17"/>
       <c r="E104" s="17"/>
@@ -9180,13 +9169,82 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
     <mergeCell ref="A99:B99"/>
     <mergeCell ref="A88:B88"/>
     <mergeCell ref="A89:B89"/>
@@ -9199,82 +9257,13 @@
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="D103:E103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9282,10 +9271,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294D100C-69AB-41F5-B732-D95ACA2B0ED1}">
-  <dimension ref="A1:F423"/>
+  <dimension ref="A1:F414"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:B70"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9549,770 +9538,819 @@
     <col min="16132" max="16133" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-    </row>
-    <row r="4" spans="1:5" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="1:6" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-    </row>
-    <row r="7" spans="1:5" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="46">
-        <v>200007197</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-    </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-    </row>
-    <row r="16" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
+    <row r="9" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+    </row>
+    <row r="11" spans="1:6" ht="24.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" s="23">
+        <v>413323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" s="23">
+        <v>-383863</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="25">
+        <v>29460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" s="31"/>
+      <c r="C16" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="F16" s="23">
+        <v>-31904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
+        <v>239</v>
+      </c>
       <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-    </row>
-    <row r="18" spans="1:6" ht="24.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="B20" s="39"/>
+      <c r="C17" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17" s="23">
+        <v>-6879</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" s="25">
+        <v>-9323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="F19" s="23">
+        <v>244236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="31"/>
       <c r="C20" s="13" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="F20" s="23">
-        <v>413323</v>
+        <v>-248991</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39" t="s">
-        <v>227</v>
-      </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="F21" s="23">
-        <v>-383863</v>
+      <c r="A21" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F21" s="25">
+        <v>-14078</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="B22" s="40"/>
+      <c r="A22" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="28"/>
       <c r="C22" s="11" t="s">
-        <v>232</v>
+        <v>260</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>233</v>
+        <v>261</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="F22" s="25">
-        <v>29460</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="F23" s="23">
-        <v>-31904</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" s="39"/>
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="B24" s="31"/>
       <c r="C24" s="13" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="F24" s="23">
-        <v>-6879</v>
+        <v>266</v>
+      </c>
+      <c r="F24" s="24">
+        <v>734</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F25" s="25">
-        <v>-9323</v>
+      <c r="A25" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="B26" s="39"/>
+      <c r="A26" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" s="31"/>
       <c r="C26" s="13" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="F26" s="23">
-        <v>244236</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
-        <v>251</v>
-      </c>
-      <c r="B27" s="39"/>
+        <v>272</v>
+      </c>
+      <c r="F26" s="24">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B27" s="31"/>
       <c r="C27" s="13" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="F27" s="23">
-        <v>-248991</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="B28" s="40"/>
+        <v>276</v>
+      </c>
+      <c r="F27" s="24">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B28" s="28"/>
       <c r="C28" s="11" t="s">
-        <v>256</v>
+        <v>28</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F28" s="25">
-        <v>-14078</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40" t="s">
-        <v>259</v>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="F29" s="25">
-        <v>1428</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="F28" s="26">
+        <v>-819</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="B31" s="39"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="F30" s="24">
+        <v>-800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" s="31"/>
       <c r="C31" s="13" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="F31" s="24">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D32" s="14" t="s">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F32" s="25">
+        <v>9719</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B34" s="31"/>
+      <c r="C34" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="F34" s="23">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35" s="23">
+        <v>7642</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="F36" s="25">
+        <v>-18917</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="31"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="F38" s="23">
+        <v>-12215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F39" s="23">
+        <v>-2077</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="B40" s="31"/>
+      <c r="C40" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="F40" s="23">
+        <v>-4625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="B41" s="28"/>
+      <c r="C41" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="F41" s="25">
+        <v>-8589</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F42" s="25">
+        <v>-22667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="F33" s="24">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="F34" s="24">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="B35" s="40"/>
-      <c r="C35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="F35" s="26">
-        <v>-819</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="F37" s="24">
-        <v>-800</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39" t="s">
-        <v>284</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="F38" s="24">
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1" ht="24.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="40" t="s">
-        <v>288</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="F41" s="25">
-        <v>9719</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>293</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="23">
-        <v>2077</v>
+      <c r="F43" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="B44" s="39"/>
+      <c r="A44" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="31"/>
       <c r="C44" s="13" t="s">
-        <v>295</v>
+        <v>53</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>296</v>
+        <v>11</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="F44" s="23">
-        <v>7642</v>
+        <v>11</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="40" t="s">
-        <v>297</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="F45" s="25">
-        <v>-18917</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="24"/>
-    </row>
-    <row r="47" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="39" t="s">
-        <v>300</v>
-      </c>
-      <c r="B47" s="39"/>
+      <c r="A45" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="B45" s="31"/>
+      <c r="C45" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="B46" s="31"/>
+      <c r="C46" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B47" s="31"/>
       <c r="C47" s="13" t="s">
-        <v>39</v>
+        <v>318</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>301</v>
+        <v>11</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="F47" s="23">
-        <v>-12215</v>
+        <v>11</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="E48" s="14" t="s">
+      <c r="A48" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="B48" s="28"/>
+      <c r="C48" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F48" s="25">
+        <v>-22667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="B49" s="31"/>
+      <c r="C49" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="23">
-        <v>-2077</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="39" t="s">
-        <v>304</v>
-      </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>305</v>
-      </c>
       <c r="E49" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="F49" s="23">
-        <v>-4625</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="F50" s="25">
-        <v>-8589</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="40" t="s">
-        <v>310</v>
-      </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="B50" s="31"/>
+      <c r="C50" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="B51" s="31"/>
+      <c r="C51" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="B52" s="31"/>
+      <c r="C52" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="F51" s="25">
+      <c r="F52" s="23">
         <v>-22667</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="39" t="s">
-        <v>313</v>
-      </c>
-      <c r="B52" s="39"/>
-      <c r="C52" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="39" t="s">
-        <v>314</v>
-      </c>
-      <c r="B53" s="39"/>
+    <row r="53" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="B53" s="31"/>
       <c r="C53" s="13" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>11</v>
+        <v>325</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="B54" s="39"/>
+        <v>326</v>
+      </c>
+      <c r="F53" s="23">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="31" t="s">
+        <v>327</v>
+      </c>
+      <c r="B54" s="31"/>
       <c r="C54" s="13" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>11</v>
@@ -10324,330 +10362,231 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="39" t="s">
-        <v>316</v>
-      </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="14" t="s">
+    <row r="55" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="B55" s="28"/>
+      <c r="C55" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="F55" s="25">
+        <v>20879</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F56" s="24">
+        <v>-1858</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="B57" s="31"/>
+      <c r="C57" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E57" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="24" t="s">
+      <c r="F57" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="39" t="s">
-        <v>317</v>
-      </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="40" t="s">
-        <v>319</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="F57" s="25">
-        <v>-22667</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="39" t="s">
-        <v>320</v>
-      </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="39" t="s">
-        <v>321</v>
-      </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="39" t="s">
-        <v>322</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F60" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="39" t="s">
-        <v>323</v>
-      </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="F61" s="23">
-        <v>-22667</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="39" t="s">
-        <v>324</v>
-      </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="F62" s="23">
-        <v>43546</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="39" t="s">
-        <v>327</v>
-      </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="40" t="s">
-        <v>328</v>
-      </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F64" s="25">
-        <v>20879</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="39" t="s">
-        <v>331</v>
-      </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="F65" s="24">
-        <v>-1858</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="39" t="s">
-        <v>334</v>
-      </c>
-      <c r="B66" s="39"/>
-      <c r="C66" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="43"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="44"/>
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-    </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="44"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-    </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="43"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+    </row>
+    <row r="60" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+    </row>
+    <row r="61" spans="1:6" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="18"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="18"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="18"/>
       <c r="C71" s="19"/>
       <c r="D71" s="20"/>
       <c r="E71" s="20"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="18"/>
       <c r="C72" s="19"/>
       <c r="D72" s="20"/>
       <c r="E72" s="20"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
       <c r="C73" s="19"/>
       <c r="D73" s="20"/>
       <c r="E73" s="20"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
       <c r="C74" s="19"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18"/>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="19"/>
       <c r="D75" s="20"/>
       <c r="E75" s="20"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="19"/>
       <c r="D76" s="20"/>
       <c r="E76" s="20"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
-      <c r="B77" s="18"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="19"/>
       <c r="D77" s="20"/>
       <c r="E77" s="20"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="18"/>
-      <c r="B78" s="18"/>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
       <c r="C78" s="19"/>
       <c r="D78" s="20"/>
       <c r="E78" s="20"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
       <c r="C79" s="19"/>
       <c r="D79" s="20"/>
       <c r="E79" s="20"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="18"/>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
       <c r="C80" s="19"/>
       <c r="D80" s="20"/>
       <c r="E80" s="20"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="18"/>
+      <c r="A81" s="19"/>
+      <c r="B81" s="19"/>
       <c r="C81" s="19"/>
       <c r="D81" s="20"/>
       <c r="E81" s="20"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="19"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
@@ -11738,65 +11677,65 @@
       <c r="E237" s="20"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238" s="19"/>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="A238" s="21"/>
+      <c r="B238" s="21"/>
+      <c r="C238" s="21"/>
       <c r="D238" s="20"/>
       <c r="E238" s="20"/>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239" s="19"/>
-      <c r="B239" s="19"/>
-      <c r="C239" s="19"/>
+      <c r="A239" s="21"/>
+      <c r="B239" s="21"/>
+      <c r="C239" s="21"/>
       <c r="D239" s="20"/>
       <c r="E239" s="20"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240" s="19"/>
-      <c r="B240" s="19"/>
-      <c r="C240" s="19"/>
+      <c r="A240" s="21"/>
+      <c r="B240" s="21"/>
+      <c r="C240" s="21"/>
       <c r="D240" s="20"/>
       <c r="E240" s="20"/>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" s="19"/>
-      <c r="B241" s="19"/>
-      <c r="C241" s="19"/>
+      <c r="A241" s="21"/>
+      <c r="B241" s="21"/>
+      <c r="C241" s="21"/>
       <c r="D241" s="20"/>
       <c r="E241" s="20"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A242" s="19"/>
-      <c r="B242" s="19"/>
-      <c r="C242" s="19"/>
+      <c r="A242" s="21"/>
+      <c r="B242" s="21"/>
+      <c r="C242" s="21"/>
       <c r="D242" s="20"/>
       <c r="E242" s="20"/>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A243" s="19"/>
-      <c r="B243" s="19"/>
-      <c r="C243" s="19"/>
+      <c r="A243" s="21"/>
+      <c r="B243" s="21"/>
+      <c r="C243" s="21"/>
       <c r="D243" s="20"/>
       <c r="E243" s="20"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244" s="19"/>
-      <c r="B244" s="19"/>
-      <c r="C244" s="19"/>
+      <c r="A244" s="21"/>
+      <c r="B244" s="21"/>
+      <c r="C244" s="21"/>
       <c r="D244" s="20"/>
       <c r="E244" s="20"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A245" s="19"/>
-      <c r="B245" s="19"/>
-      <c r="C245" s="19"/>
+      <c r="A245" s="21"/>
+      <c r="B245" s="21"/>
+      <c r="C245" s="21"/>
       <c r="D245" s="20"/>
       <c r="E245" s="20"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A246" s="19"/>
-      <c r="B246" s="19"/>
-      <c r="C246" s="19"/>
+      <c r="A246" s="21"/>
+      <c r="B246" s="21"/>
+      <c r="C246" s="21"/>
       <c r="D246" s="20"/>
       <c r="E246" s="20"/>
     </row>
@@ -12721,131 +12660,113 @@
       <c r="A378" s="21"/>
       <c r="B378" s="21"/>
       <c r="C378" s="21"/>
-      <c r="D378" s="20"/>
-      <c r="E378" s="20"/>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" s="21"/>
       <c r="B379" s="21"/>
       <c r="C379" s="21"/>
-      <c r="D379" s="20"/>
-      <c r="E379" s="20"/>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="21"/>
       <c r="B380" s="21"/>
       <c r="C380" s="21"/>
-      <c r="D380" s="20"/>
-      <c r="E380" s="20"/>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" s="21"/>
       <c r="B381" s="21"/>
       <c r="C381" s="21"/>
-      <c r="D381" s="20"/>
-      <c r="E381" s="20"/>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" s="21"/>
       <c r="B382" s="21"/>
       <c r="C382" s="21"/>
-      <c r="D382" s="20"/>
-      <c r="E382" s="20"/>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" s="21"/>
       <c r="B383" s="21"/>
       <c r="C383" s="21"/>
-      <c r="D383" s="20"/>
-      <c r="E383" s="20"/>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" s="21"/>
       <c r="B384" s="21"/>
       <c r="C384" s="21"/>
-      <c r="D384" s="20"/>
-      <c r="E384" s="20"/>
-    </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="21"/>
       <c r="B385" s="21"/>
       <c r="C385" s="21"/>
-      <c r="D385" s="20"/>
-      <c r="E385" s="20"/>
-    </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" s="21"/>
       <c r="B386" s="21"/>
       <c r="C386" s="21"/>
-      <c r="D386" s="20"/>
-      <c r="E386" s="20"/>
-    </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" s="21"/>
       <c r="B387" s="21"/>
       <c r="C387" s="21"/>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" s="21"/>
       <c r="B388" s="21"/>
       <c r="C388" s="21"/>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" s="21"/>
       <c r="B389" s="21"/>
       <c r="C389" s="21"/>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" s="21"/>
       <c r="B390" s="21"/>
       <c r="C390" s="21"/>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" s="21"/>
       <c r="B391" s="21"/>
       <c r="C391" s="21"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="21"/>
       <c r="B392" s="21"/>
       <c r="C392" s="21"/>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="21"/>
       <c r="B393" s="21"/>
       <c r="C393" s="21"/>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" s="21"/>
       <c r="B394" s="21"/>
       <c r="C394" s="21"/>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" s="21"/>
       <c r="B395" s="21"/>
       <c r="C395" s="21"/>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" s="21"/>
       <c r="B396" s="21"/>
       <c r="C396" s="21"/>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="21"/>
       <c r="B397" s="21"/>
       <c r="C397" s="21"/>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" s="21"/>
       <c r="B398" s="21"/>
       <c r="C398" s="21"/>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" s="21"/>
       <c r="B399" s="21"/>
       <c r="C399" s="21"/>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" s="21"/>
       <c r="B400" s="21"/>
       <c r="C400" s="21"/>
@@ -12920,83 +12841,42 @@
       <c r="B414" s="21"/>
       <c r="C414" s="21"/>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A415" s="21"/>
-      <c r="B415" s="21"/>
-      <c r="C415" s="21"/>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A416" s="21"/>
-      <c r="B416" s="21"/>
-      <c r="C416" s="21"/>
-    </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A417" s="21"/>
-      <c r="B417" s="21"/>
-      <c r="C417" s="21"/>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A418" s="21"/>
-      <c r="B418" s="21"/>
-      <c r="C418" s="21"/>
-    </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A419" s="21"/>
-      <c r="B419" s="21"/>
-      <c r="C419" s="21"/>
-    </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A420" s="21"/>
-      <c r="B420" s="21"/>
-      <c r="C420" s="21"/>
-    </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A421" s="21"/>
-      <c r="B421" s="21"/>
-      <c r="C421" s="21"/>
-    </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A422" s="21"/>
-      <c r="B422" s="21"/>
-      <c r="C422" s="21"/>
-    </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A423" s="21"/>
-      <c r="B423" s="21"/>
-      <c r="C423" s="21"/>
-    </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A46:B46"/>
+  <mergeCells count="59">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
@@ -13005,36 +12885,23 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>